<commit_message>
Multiple key checks per frame
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\source\repos\Raycaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{C31F3E24-2844-40B7-B358-913D2D5ADDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463E5268-53EE-4B06-A3DC-F393BA7C0B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="195" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="28680" yWindow="195" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>CPU without textures</t>
   </si>
@@ -64,11 +64,14 @@
   <si>
     <t>FPS</t>
   </si>
+  <si>
+    <t>Python3 (second year)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -281,22 +284,25 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>Python3 (second year)</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>CPU without textures</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>CPU with textures</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>GPU without textures</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>GPU with textures</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>GPU with texture object</c:v>
                 </c:pt>
               </c:strCache>
@@ -304,23 +310,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>267</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>234</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>349</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>338</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>347</c:v>
                 </c:pt>
               </c:numCache>
@@ -669,22 +678,25 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>Python3 (second year)</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>CPU without textures</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>CPU with textures</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>GPU without textures</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>GPU with textures</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>GPU with texture object</c:v>
                 </c:pt>
               </c:strCache>
@@ -692,23 +704,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:f>Sheet1!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>289</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>252</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>350</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>337</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>346</c:v>
                 </c:pt>
               </c:numCache>
@@ -972,7 +987,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$25</c:f>
+              <c:f>Sheet1!$B$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1007,7 +1022,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$26:$A$35</c:f>
+              <c:f>Sheet1!$A$27:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1046,7 +1061,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$26:$B$35</c:f>
+              <c:f>Sheet1!$B$27:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3029,13 +3044,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3065,13 +3080,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3101,13 +3116,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1257300</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3452,11 +3467,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3476,153 +3491,164 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>267</v>
+        <v>11</v>
       </c>
       <c r="C2">
-        <v>289</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>234</v>
+        <v>267</v>
       </c>
       <c r="C3">
-        <v>252</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>349</v>
+        <v>234</v>
       </c>
       <c r="C4">
-        <v>350</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="C5">
-        <v>337</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>338</v>
+      </c>
+      <c r="C6">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>347</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>346</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="B26">
-        <v>243</v>
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>A26*2</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B27">
-        <v>290</v>
+        <v>243</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>A27*2</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B28">
-        <v>322</v>
+        <v>290</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>A28*2</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B29">
-        <v>342</v>
+        <v>322</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>A29*2</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B30">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>A30*2</f>
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="B31">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" ref="A32:A34" si="0">A31*2</f>
-        <v>128</v>
+        <f>A31*2</f>
+        <v>64</v>
       </c>
       <c r="B32">
-        <v>341</v>
+        <v>346</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="0"/>
-        <v>256</v>
+        <f t="shared" ref="A33:A35" si="0">A32*2</f>
+        <v>128</v>
       </c>
       <c r="B33">
-        <v>336</v>
+        <v>341</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
-        <v>512</v>
+        <v>256</v>
       </c>
       <c r="B34">
-        <v>318</v>
+        <v>336</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>A34*2</f>
+        <f t="shared" si="0"/>
+        <v>512</v>
+      </c>
+      <c r="B35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f>A35*2</f>
         <v>1024</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>292</v>
       </c>
     </row>

</xml_diff>